<commit_message>
defend -> defence 이름 변경, 스탯 추가
</commit_message>
<xml_diff>
--- a/XLSX/TowerTable.xlsx
+++ b/XLSX/TowerTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CProject\SProject\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AC0280-7F15-42C7-9CD2-5B3CA6A5182D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1F6269-98B8-42D6-96E8-5797860FE5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
+    <workbookView xWindow="7080" yWindow="4230" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
   </bookViews>
   <sheets>
     <sheet name="!NormalTower" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="56">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Defend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Hp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -237,6 +233,14 @@
   </si>
   <si>
     <t>class&lt;AUnitStageTower&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defend는 방어하다, 동사격 의미임으로 Defence로 변경</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -642,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3F3863-F070-4592-A50F-8035B6750A51}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -690,87 +694,87 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -787,10 +791,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -820,10 +824,10 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -840,10 +844,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
       </c>
       <c r="G4">
         <v>6</v>
@@ -873,10 +877,10 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -893,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -926,10 +930,10 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -946,10 +950,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G12" si="0">ROUND(G5*1.1,0)</f>
@@ -980,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1000,10 +1004,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -1034,10 +1038,10 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1054,10 +1058,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -1088,10 +1092,10 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1108,10 +1112,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
         <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -1142,10 +1146,10 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1162,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -1196,10 +1200,10 @@
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1216,10 +1220,10 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
         <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -1250,10 +1254,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1270,10 +1274,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
         <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -1304,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1326,10 +1330,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
       </c>
       <c r="G13">
         <v>40</v>
@@ -1359,10 +1363,10 @@
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1381,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
         <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
       </c>
       <c r="G14">
         <f t="shared" ref="G14" si="3">ROUND(G13*1.1,0)</f>
@@ -1415,10 +1419,10 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -1437,10 +1441,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
         <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>23</v>
       </c>
       <c r="G15">
         <f t="shared" ref="G15" si="4">ROUND(G14*1.1,0)</f>
@@ -1471,10 +1475,10 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -1493,10 +1497,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
         <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
       </c>
       <c r="G16">
         <f t="shared" ref="G16" si="5">ROUND(G15*1.1,0)</f>
@@ -1527,10 +1531,10 @@
         <v>1</v>
       </c>
       <c r="P16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -1549,10 +1553,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
         <v>22</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
       </c>
       <c r="G17">
         <f>ROUND(G16*1.1,0)</f>
@@ -1583,10 +1587,10 @@
         <v>1</v>
       </c>
       <c r="P17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -1605,10 +1609,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
         <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18" si="6">ROUND(G17*1.1,0)</f>
@@ -1639,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -1661,10 +1665,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
         <v>22</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
       </c>
       <c r="G19">
         <f t="shared" ref="G19" si="7">ROUND(G18*1.1,0)</f>
@@ -1695,10 +1699,10 @@
         <v>1</v>
       </c>
       <c r="P19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -1717,10 +1721,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
         <v>22</v>
-      </c>
-      <c r="F20" t="s">
-        <v>23</v>
       </c>
       <c r="G20">
         <f t="shared" ref="G20" si="8">ROUND(G19*1.1,0)</f>
@@ -1751,10 +1755,10 @@
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -1773,10 +1777,10 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
         <v>22</v>
-      </c>
-      <c r="F21" t="s">
-        <v>23</v>
       </c>
       <c r="G21">
         <f t="shared" ref="G21" si="9">ROUND(G20*1.1,0)</f>
@@ -1807,10 +1811,10 @@
         <v>1</v>
       </c>
       <c r="P21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -1829,10 +1833,10 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
         <v>22</v>
-      </c>
-      <c r="F22" t="s">
-        <v>23</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22" si="10">ROUND(G21*1.1,0)</f>
@@ -1863,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -1885,10 +1889,10 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
         <v>24</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
       </c>
       <c r="G23">
         <v>30</v>
@@ -1918,10 +1922,10 @@
         <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -1940,10 +1944,10 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
         <v>24</v>
-      </c>
-      <c r="F24" t="s">
-        <v>25</v>
       </c>
       <c r="G24">
         <f t="shared" ref="G24" si="11">ROUND(G23*1.1,0)</f>
@@ -1974,10 +1978,10 @@
         <v>1</v>
       </c>
       <c r="P24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -1996,10 +2000,10 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
         <v>24</v>
-      </c>
-      <c r="F25" t="s">
-        <v>25</v>
       </c>
       <c r="G25">
         <f t="shared" ref="G25" si="12">ROUND(G24*1.1,0)</f>
@@ -2030,10 +2034,10 @@
         <v>1</v>
       </c>
       <c r="P25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -2052,10 +2056,10 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
         <v>24</v>
-      </c>
-      <c r="F26" t="s">
-        <v>25</v>
       </c>
       <c r="G26">
         <f t="shared" ref="G26" si="13">ROUND(G25*1.1,0)</f>
@@ -2086,10 +2090,10 @@
         <v>1</v>
       </c>
       <c r="P26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2108,10 +2112,10 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
         <v>24</v>
-      </c>
-      <c r="F27" t="s">
-        <v>25</v>
       </c>
       <c r="G27">
         <f t="shared" ref="G27" si="14">ROUND(G26*1.1,0)</f>
@@ -2142,10 +2146,10 @@
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2164,10 +2168,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
         <v>24</v>
-      </c>
-      <c r="F28" t="s">
-        <v>25</v>
       </c>
       <c r="G28">
         <f t="shared" ref="G28" si="15">ROUND(G27*1.1,0)</f>
@@ -2198,10 +2202,10 @@
         <v>1</v>
       </c>
       <c r="P28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2220,10 +2224,10 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="s">
         <v>24</v>
-      </c>
-      <c r="F29" t="s">
-        <v>25</v>
       </c>
       <c r="G29">
         <f t="shared" ref="G29" si="16">ROUND(G28*1.1,0)</f>
@@ -2254,10 +2258,10 @@
         <v>1</v>
       </c>
       <c r="P29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2276,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" t="s">
         <v>24</v>
-      </c>
-      <c r="F30" t="s">
-        <v>25</v>
       </c>
       <c r="G30">
         <f t="shared" ref="G30" si="17">ROUND(G29*1.1,0)</f>
@@ -2310,10 +2314,10 @@
         <v>1</v>
       </c>
       <c r="P30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2332,10 +2336,10 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" t="s">
         <v>24</v>
-      </c>
-      <c r="F31" t="s">
-        <v>25</v>
       </c>
       <c r="G31">
         <f t="shared" ref="G31" si="18">ROUND(G30*1.1,0)</f>
@@ -2366,10 +2370,10 @@
         <v>1</v>
       </c>
       <c r="P31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2388,10 +2392,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" t="s">
         <v>24</v>
-      </c>
-      <c r="F32" t="s">
-        <v>25</v>
       </c>
       <c r="G32">
         <f t="shared" ref="G32:G38" si="19">ROUND(G31*1.1,0)</f>
@@ -2422,10 +2426,10 @@
         <v>1</v>
       </c>
       <c r="P32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -2444,10 +2448,10 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
         <v>26</v>
-      </c>
-      <c r="F33" t="s">
-        <v>27</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2477,10 +2481,10 @@
         <v>0</v>
       </c>
       <c r="P33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -2499,10 +2503,10 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
         <v>26</v>
-      </c>
-      <c r="F34" t="s">
-        <v>27</v>
       </c>
       <c r="G34">
         <f t="shared" si="19"/>
@@ -2533,10 +2537,10 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -2555,10 +2559,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
         <v>26</v>
-      </c>
-      <c r="F35" t="s">
-        <v>27</v>
       </c>
       <c r="G35">
         <f t="shared" si="19"/>
@@ -2589,10 +2593,10 @@
         <v>0</v>
       </c>
       <c r="P35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -2611,10 +2615,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
         <v>26</v>
-      </c>
-      <c r="F36" t="s">
-        <v>27</v>
       </c>
       <c r="G36">
         <f t="shared" si="19"/>
@@ -2645,10 +2649,10 @@
         <v>0</v>
       </c>
       <c r="P36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -2667,10 +2671,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" t="s">
         <v>26</v>
-      </c>
-      <c r="F37" t="s">
-        <v>27</v>
       </c>
       <c r="G37">
         <f t="shared" si="19"/>
@@ -2701,10 +2705,10 @@
         <v>0</v>
       </c>
       <c r="P37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -2723,10 +2727,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
         <v>26</v>
-      </c>
-      <c r="F38" t="s">
-        <v>27</v>
       </c>
       <c r="G38">
         <f t="shared" si="19"/>
@@ -2757,10 +2761,10 @@
         <v>0</v>
       </c>
       <c r="P38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2771,135 +2775,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F27775-B38A-425D-9D8A-9CD959A261C6}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
StageTowerUnit 기본 베이스 추가
</commit_message>
<xml_diff>
--- a/XLSX/TowerTable.xlsx
+++ b/XLSX/TowerTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CProject\SProject\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1F6269-98B8-42D6-96E8-5797860FE5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260DA1BA-C497-48A5-94C6-E50B9F669463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="4230" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
   </bookViews>
   <sheets>
     <sheet name="!NormalTower" sheetId="1" r:id="rId1"/>
@@ -232,15 +232,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>class&lt;AUnitStageTower&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Defence</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Defend는 방어하다, 동사격 의미임으로 Defence로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class&lt;AStageTowerUnit&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3F3863-F070-4592-A50F-8035B6750A51}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -694,7 +694,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -771,7 +771,7 @@
         <v>44</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>18</v>
@@ -2777,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F27775-B38A-425D-9D8A-9CD959A261C6}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2837,13 +2837,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>